<commit_message>
Update Py folder from hackathon-2 (no branch merge)
</commit_message>
<xml_diff>
--- a/Py/DI-Bootcamp/Week7/Day3/Daily/Dino File Filtered.xlsx
+++ b/Py/DI-Bootcamp/Week7/Day3/Daily/Dino File Filtered.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dianatalis/Desktop/DevelopersInt/Py/DI-Bootcamp/Week7/Day3/Daily/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{465254A2-F0B1-A540-AA45-DBC62DE46811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A8C62B5-300E-B040-9685-D07FEBF85EB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Part 1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,20 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Part 2'!$A$1:$K$29</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Part 3'!$A$1:$T$29</definedName>
   </definedNames>
-  <calcPr calcId="124519" iterateDelta="9.9999999999999995E-7"/>
+  <calcPr calcId="191029" iterateDelta="9.9999999999999995E-7"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1899,7 +1912,7 @@
   <dimension ref="A1:T38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G49" sqref="G49"/>
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2940,7 +2953,7 @@
       <c r="S32" s="8"/>
       <c r="T32" s="8"/>
     </row>
-    <row r="33" spans="14:20" x14ac:dyDescent="0.2">
+    <row r="33" spans="7:20" x14ac:dyDescent="0.2">
       <c r="N33" s="8"/>
       <c r="O33" s="8"/>
       <c r="P33" s="8"/>
@@ -2949,7 +2962,7 @@
       <c r="S33" s="8"/>
       <c r="T33" s="8"/>
     </row>
-    <row r="34" spans="14:20" x14ac:dyDescent="0.2">
+    <row r="34" spans="7:20" x14ac:dyDescent="0.2">
       <c r="N34" s="8"/>
       <c r="O34" s="8"/>
       <c r="P34" s="8"/>
@@ -2958,7 +2971,7 @@
       <c r="S34" s="8"/>
       <c r="T34" s="8"/>
     </row>
-    <row r="35" spans="14:20" x14ac:dyDescent="0.2">
+    <row r="35" spans="7:20" x14ac:dyDescent="0.2">
       <c r="N35" s="8"/>
       <c r="O35" s="8"/>
       <c r="P35" s="8"/>
@@ -2967,7 +2980,7 @@
       <c r="S35" s="8"/>
       <c r="T35" s="8"/>
     </row>
-    <row r="36" spans="14:20" x14ac:dyDescent="0.2">
+    <row r="36" spans="7:20" x14ac:dyDescent="0.2">
       <c r="N36" s="8"/>
       <c r="O36" s="8"/>
       <c r="P36" s="8"/>
@@ -2976,7 +2989,7 @@
       <c r="S36" s="8"/>
       <c r="T36" s="8"/>
     </row>
-    <row r="37" spans="14:20" x14ac:dyDescent="0.2">
+    <row r="37" spans="7:20" x14ac:dyDescent="0.2">
       <c r="N37" s="8"/>
       <c r="O37" s="8"/>
       <c r="P37" s="8"/>
@@ -2985,7 +2998,11 @@
       <c r="S37" s="8"/>
       <c r="T37" s="8"/>
     </row>
-    <row r="38" spans="14:20" x14ac:dyDescent="0.2">
+    <row r="38" spans="7:20" x14ac:dyDescent="0.2">
+      <c r="G38" s="1">
+        <f>MEDIAN(F:F)</f>
+        <v>6.5</v>
+      </c>
       <c r="N38" s="8"/>
       <c r="O38" s="8"/>
       <c r="P38" s="8"/>

</xml_diff>